<commit_message>
add test that student dropping class has no effect
</commit_message>
<xml_diff>
--- a/tests/component/update_student_sheets/test_cases/there_is_already_data/teacher.xlsx
+++ b/tests/component/update_student_sheets/test_cases/there_is_already_data/teacher.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjsha\Documents\Git\student-teacher-gradebook\tests\component\update_student_sheets\test_cases\there_is_already_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39154F4C-3918-4772-AA9B-3EF6BAF16ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F8B281-965D-4C6A-B9D1-714D1FC9C4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="5" xr2:uid="{1C66C71B-6ED8-4699-9FB2-CB3156D48D4F}"/>
+    <workbookView xWindow="23880" yWindow="2895" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{1C66C71B-6ED8-4699-9FB2-CB3156D48D4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Student</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>Mus476_John Doe_gradebook.xlsx</t>
-  </si>
-  <si>
-    <t>b7b5a7e9</t>
-  </si>
-  <si>
-    <t>Mus476_Molly Doe_gradebook.xlsx</t>
   </si>
   <si>
     <t>9e2aaa00</t>
@@ -175,8 +169,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA661278-7CA3-4F00-B615-A260AC448CE7}" name="Table1" displayName="Table1" ref="A1:F100" totalsRowShown="0">
-  <autoFilter ref="A1:F100" xr:uid="{DA661278-7CA3-4F00-B615-A260AC448CE7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DA661278-7CA3-4F00-B615-A260AC448CE7}" name="Table1" displayName="Table1" ref="A1:F99" totalsRowShown="0">
+  <autoFilter ref="A1:F99" xr:uid="{DA661278-7CA3-4F00-B615-A260AC448CE7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D55A0BF3-7770-4469-9934-4DCD2E97513E}" name="ID"/>
     <tableColumn id="7" xr3:uid="{7F32FE12-7E5E-4589-82CF-1E1BA733C019}" name="Student"/>
@@ -516,7 +510,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -530,16 +524,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0FBE7F-C5A8-44D7-BCA4-446189B2A194}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -581,21 +575,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -623,10 +606,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>27</v>
@@ -744,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39084932-C412-4582-9044-67EC2A697005}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -758,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1">
         <v>98</v>
@@ -769,7 +752,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -780,7 +763,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>68</v>

</xml_diff>